<commit_message>
Maj DD et DF
</commit_message>
<xml_diff>
--- a/Dépendance Fonctionnel.xlsx
+++ b/Dépendance Fonctionnel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>ID potion</t>
   </si>
@@ -88,15 +88,9 @@
     <t xml:space="preserve">Quantité récipient </t>
   </si>
   <si>
-    <t>Prix récipient</t>
-  </si>
-  <si>
     <t>ID commande</t>
   </si>
   <si>
-    <t xml:space="preserve">Potion </t>
-  </si>
-  <si>
     <t>Type récipient</t>
   </si>
   <si>
@@ -106,15 +100,9 @@
     <t>Prix totale</t>
   </si>
   <si>
-    <t>Onguent</t>
-  </si>
-  <si>
     <t>Quantité onguent</t>
   </si>
   <si>
-    <t>Ingrédient</t>
-  </si>
-  <si>
     <t>Fraicheur</t>
   </si>
   <si>
@@ -128,6 +116,33 @@
   </si>
   <si>
     <t>Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom Potion </t>
+  </si>
+  <si>
+    <t>Nom Onguent</t>
+  </si>
+  <si>
+    <t>Nom Ingrédient</t>
+  </si>
+  <si>
+    <t>ID Client</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
+    <t>N° Commande</t>
+  </si>
+  <si>
+    <t>Prenom client</t>
+  </si>
+  <si>
+    <t>ID ingrédient (stock)</t>
   </si>
 </sst>
 </file>
@@ -159,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,11 +182,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,14 +212,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -197,10 +221,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,40 +547,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W80"/>
+  <dimension ref="B2:W87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5546875" defaultRowHeight="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" style="8"/>
-    <col min="3" max="3" width="17" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="6"/>
+    <col min="3" max="3" width="17" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
         <v>16</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="9">
         <v>24</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="9">
         <v>28</v>
       </c>
-      <c r="H2" s="1">
-        <v>35</v>
-      </c>
-      <c r="I2" s="1">
-        <v>47</v>
-      </c>
-      <c r="J2" s="1"/>
+      <c r="H2" s="9">
+        <v>41</v>
+      </c>
+      <c r="I2" s="9">
+        <v>54</v>
+      </c>
+      <c r="J2" s="9">
+        <v>58</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -556,21 +598,21 @@
       <c r="W2" s="1"/>
     </row>
     <row r="3" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -580,21 +622,21 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -604,21 +646,21 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7">
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -628,23 +670,23 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -654,23 +696,23 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -680,23 +722,23 @@
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -706,23 +748,23 @@
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+      <c r="B9" s="10">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -732,23 +774,23 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+      <c r="B10" s="10">
         <v>8</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -758,23 +800,23 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7">
+      <c r="B11" s="10">
         <v>9</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -784,23 +826,23 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -810,23 +852,23 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -836,23 +878,23 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7">
+      <c r="B14" s="10">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -862,23 +904,23 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7">
+      <c r="B15" s="10">
         <v>13</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -888,21 +930,21 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="2:23" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7">
+      <c r="B16" s="10">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -912,21 +954,21 @@
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7">
+      <c r="B17" s="10">
         <v>15</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -936,21 +978,21 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
+      <c r="B18" s="7">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -960,21 +1002,21 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="7">
+      <c r="B19" s="10">
         <v>17</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -984,23 +1026,23 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7">
+      <c r="B20" s="10">
         <v>18</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1010,23 +1052,23 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7">
+      <c r="B21" s="10">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1036,23 +1078,23 @@
       <c r="Q21" s="1"/>
     </row>
     <row r="22" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="7">
+      <c r="B22" s="10">
         <v>20</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>1</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1062,23 +1104,23 @@
       <c r="Q22" s="1"/>
     </row>
     <row r="23" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7">
+      <c r="B23" s="10">
         <v>21</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1088,23 +1130,23 @@
       <c r="Q23" s="1"/>
     </row>
     <row r="24" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="7">
+      <c r="B24" s="10">
         <v>22</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1114,21 +1156,21 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="7">
+      <c r="B25" s="10">
         <v>23</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1138,21 +1180,21 @@
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6">
+      <c r="B26" s="7">
         <v>24</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1162,21 +1204,21 @@
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="7">
+      <c r="B27" s="10">
         <v>25</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1186,21 +1228,21 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7">
+      <c r="B28" s="10">
         <v>26</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2">
-        <v>1</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1210,21 +1252,21 @@
       <c r="Q28" s="1"/>
     </row>
     <row r="29" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="7">
+      <c r="B29" s="10">
         <v>27</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1234,23 +1276,23 @@
       <c r="Q29" s="1"/>
     </row>
     <row r="30" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="6">
+      <c r="B30" s="7">
         <v>28</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="C30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9">
+        <v>1</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -1260,20 +1302,21 @@
       <c r="Q30" s="1"/>
     </row>
     <row r="31" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="7">
+      <c r="B31" s="10">
         <v>29</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="9">
+        <v>1</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1283,20 +1326,21 @@
       <c r="Q31" s="1"/>
     </row>
     <row r="32" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
+      <c r="B32" s="10">
         <v>30</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="9">
+        <v>1</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1306,20 +1350,21 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="7">
+      <c r="B33" s="10">
         <v>31</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="9">
+        <v>1</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -1329,21 +1374,21 @@
       <c r="Q33" s="1"/>
     </row>
     <row r="34" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="7">
+      <c r="B34" s="10">
         <v>32</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9">
+        <v>1</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -1353,21 +1398,21 @@
       <c r="Q34" s="1"/>
     </row>
     <row r="35" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="7">
+      <c r="B35" s="10">
         <v>33</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <v>1</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -1377,21 +1422,23 @@
       <c r="Q35" s="1"/>
     </row>
     <row r="36" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="7">
+      <c r="B36" s="10">
         <v>34</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="C36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9">
+        <v>1</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9">
+        <v>1</v>
+      </c>
+      <c r="J36" s="9"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -1401,21 +1448,21 @@
       <c r="Q36" s="1"/>
     </row>
     <row r="37" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6">
+      <c r="B37" s="10">
         <v>35</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="C37" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9">
+        <v>1</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -1425,23 +1472,21 @@
       <c r="Q37" s="1"/>
     </row>
     <row r="38" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="7">
+      <c r="B38" s="10">
         <v>36</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="2">
-        <v>1</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="C38" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9">
+        <v>1</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -1451,21 +1496,21 @@
       <c r="Q38" s="1"/>
     </row>
     <row r="39" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="7">
+      <c r="B39" s="10">
         <v>37</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="2">
-        <v>1</v>
-      </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="C39" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9">
+        <v>1</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -1475,21 +1520,21 @@
       <c r="Q39" s="1"/>
     </row>
     <row r="40" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="7">
+      <c r="B40" s="10">
         <v>38</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="2">
-        <v>1</v>
-      </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="C40" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9">
+        <v>1</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -1499,23 +1544,21 @@
       <c r="Q40" s="1"/>
     </row>
     <row r="41" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="7">
+      <c r="B41" s="10">
         <v>39</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="2">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="C41" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9">
+        <v>1</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -1525,21 +1568,21 @@
       <c r="Q41" s="1"/>
     </row>
     <row r="42" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="7">
+      <c r="B42" s="10">
         <v>40</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="2">
-        <v>1</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="C42" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -1552,20 +1595,18 @@
       <c r="B43" s="7">
         <v>41</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="H43" s="2">
-        <v>1</v>
-      </c>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -1575,23 +1616,23 @@
       <c r="Q43" s="1"/>
     </row>
     <row r="44" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="7">
+      <c r="B44" s="10">
         <v>42</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="C44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -1601,21 +1642,21 @@
       <c r="Q44" s="1"/>
     </row>
     <row r="45" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="7">
+      <c r="B45" s="10">
         <v>43</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="2">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="C45" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -1625,23 +1666,21 @@
       <c r="Q45" s="1"/>
     </row>
     <row r="46" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="7">
+      <c r="B46" s="10">
         <v>44</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="2">
-        <v>1</v>
-      </c>
-      <c r="I46" s="1">
-        <v>1</v>
-      </c>
-      <c r="J46" s="1"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -1651,21 +1690,23 @@
       <c r="Q46" s="1"/>
     </row>
     <row r="47" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="7">
+      <c r="B47" s="10">
         <v>45</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="2">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
+      <c r="C47" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -1675,21 +1716,21 @@
       <c r="Q47" s="1"/>
     </row>
     <row r="48" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="7">
+      <c r="B48" s="10">
         <v>46</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="2">
-        <v>1</v>
-      </c>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
+      <c r="C48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -1699,21 +1740,23 @@
       <c r="Q48" s="1"/>
     </row>
     <row r="49" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="6">
+      <c r="B49" s="10">
         <v>47</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1" t="s">
+      <c r="C49" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J49" s="1"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -1723,21 +1766,23 @@
       <c r="Q49" s="1"/>
     </row>
     <row r="50" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="7">
+      <c r="B50" s="10">
         <v>48</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="2">
-        <v>1</v>
-      </c>
-      <c r="J50" s="1"/>
+      <c r="C50" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9">
+        <v>1</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -1747,21 +1792,21 @@
       <c r="Q50" s="1"/>
     </row>
     <row r="51" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="7">
+      <c r="B51" s="10">
         <v>49</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="2">
-        <v>1</v>
-      </c>
-      <c r="J51" s="1"/>
+      <c r="C51" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9">
+        <v>1</v>
+      </c>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -1771,21 +1816,23 @@
       <c r="Q51" s="1"/>
     </row>
     <row r="52" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="7">
+      <c r="B52" s="10">
         <v>50</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="2">
-        <v>1</v>
-      </c>
-      <c r="J52" s="1"/>
+      <c r="C52" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9">
+        <v>1</v>
+      </c>
+      <c r="I52" s="9">
+        <v>1</v>
+      </c>
+      <c r="J52" s="9"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -1795,7 +1842,23 @@
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J53" s="1"/>
+      <c r="B53" s="10">
+        <v>51</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9">
+        <v>1</v>
+      </c>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9">
+        <v>1</v>
+      </c>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -1805,15 +1868,23 @@
       <c r="Q53" s="1"/>
     </row>
     <row r="54" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="7"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
+      <c r="B54" s="10">
+        <v>52</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9">
+        <v>1</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9">
+        <v>1</v>
+      </c>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -1823,15 +1894,23 @@
       <c r="Q54" s="1"/>
     </row>
     <row r="55" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="7"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
+      <c r="B55" s="10">
+        <v>53</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9">
+        <v>1</v>
+      </c>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9">
+        <v>1</v>
+      </c>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -1841,15 +1920,21 @@
       <c r="Q55" s="1"/>
     </row>
     <row r="56" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="7"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
+      <c r="B56" s="7">
+        <v>54</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J56" s="9"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -1859,15 +1944,21 @@
       <c r="Q56" s="1"/>
     </row>
     <row r="57" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="7"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
+      <c r="B57" s="10">
+        <v>55</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9">
+        <v>1</v>
+      </c>
+      <c r="J57" s="9"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -1877,15 +1968,21 @@
       <c r="Q57" s="1"/>
     </row>
     <row r="58" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="7"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
+      <c r="B58" s="10">
+        <v>56</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9">
+        <v>1</v>
+      </c>
+      <c r="J58" s="9"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -1895,15 +1992,21 @@
       <c r="Q58" s="1"/>
     </row>
     <row r="59" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="7"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
+      <c r="B59" s="10">
+        <v>57</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9">
+        <v>1</v>
+      </c>
+      <c r="J59" s="9"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -1913,13 +2016,21 @@
       <c r="Q59" s="1"/>
     </row>
     <row r="60" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
+      <c r="B60" s="7">
+        <v>58</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -1929,13 +2040,21 @@
       <c r="Q60" s="1"/>
     </row>
     <row r="61" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
+      <c r="B61" s="10">
+        <v>59</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9">
+        <v>1</v>
+      </c>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -1945,13 +2064,21 @@
       <c r="Q61" s="1"/>
     </row>
     <row r="62" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
+      <c r="B62" s="10">
+        <v>60</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9">
+        <v>1</v>
+      </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -1961,13 +2088,21 @@
       <c r="Q62" s="1"/>
     </row>
     <row r="63" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
+      <c r="B63" s="10">
+        <v>61</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9">
+        <v>1</v>
+      </c>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -1977,13 +2112,21 @@
       <c r="Q63" s="1"/>
     </row>
     <row r="64" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
+      <c r="B64" s="10">
+        <v>62</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9">
+        <v>1</v>
+      </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -1992,10 +2135,12 @@
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
     </row>
-    <row r="65" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+    <row r="65" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="5"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -2008,10 +2153,12 @@
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
     </row>
-    <row r="66" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
+    <row r="66" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="5"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -2024,7 +2171,7 @@
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -2040,7 +2187,7 @@
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
     </row>
-    <row r="68" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -2056,7 +2203,7 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -2072,7 +2219,7 @@
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
     </row>
-    <row r="70" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -2088,7 +2235,7 @@
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
     </row>
-    <row r="71" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -2104,7 +2251,7 @@
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
     </row>
-    <row r="72" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -2120,7 +2267,7 @@
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
     </row>
-    <row r="73" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -2136,7 +2283,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -2152,7 +2299,7 @@
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
     </row>
-    <row r="75" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -2168,7 +2315,7 @@
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
     </row>
-    <row r="76" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -2184,7 +2331,7 @@
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
     </row>
-    <row r="77" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -2200,7 +2347,7 @@
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
     </row>
-    <row r="78" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -2216,7 +2363,7 @@
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
     </row>
-    <row r="79" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -2232,7 +2379,7 @@
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
     </row>
-    <row r="80" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -2248,6 +2395,118 @@
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
     </row>
+    <row r="81" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+    </row>
+    <row r="82" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+    </row>
+    <row r="83" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+    </row>
+    <row r="84" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+      <c r="Q84" s="1"/>
+    </row>
+    <row r="85" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+      <c r="O85" s="1"/>
+      <c r="P85" s="1"/>
+      <c r="Q85" s="1"/>
+    </row>
+    <row r="86" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+    </row>
+    <row r="87" spans="4:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>